<commit_message>
daily 20-01-2021 51 tareas terminadas
</commit_message>
<xml_diff>
--- a/Registro_deActividades.xlsx
+++ b/Registro_deActividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaito\Desktop\Semestre-2021-1\1645-Diseno_Digital_Moderno_2021-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FE7F78-A36E-4215-AE7D-82D26623BDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9BBF5D-462A-4591-A499-E58D2AAFE661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="18900" windowHeight="11160" xr2:uid="{49A6EE8B-1464-4CCF-A474-1FC1C12E61EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{49A6EE8B-1464-4CCF-A474-1FC1C12E61EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
   <si>
     <t>Kambalam</t>
   </si>
@@ -259,12 +259,6 @@
     <t>osc 55 y con not</t>
   </si>
   <si>
-    <t>que sig jk</t>
-  </si>
-  <si>
-    <t>ff´s rs con nand</t>
-  </si>
-  <si>
     <t>Control de palabras de 8 bits (8 tiempos)</t>
   </si>
   <si>
@@ -308,6 +302,21 @@
   </si>
   <si>
     <t>Diseñar un comparador de dos palabras A y B de 4 bits cada una y que detecte cuando A y B son iguales</t>
+  </si>
+  <si>
+    <t>Como funciona un flip flop rs con compuertas nand</t>
+  </si>
+  <si>
+    <t>Como se implementa un tren de pulsos con un 555</t>
+  </si>
+  <si>
+    <t>Oscilador con compertas not</t>
+  </si>
+  <si>
+    <t>¿Qué significa la JK en el flip flop JK?</t>
+  </si>
+  <si>
+    <t>Diseñar un multiplicador x5 de un dígito en BCD.Se desea implementación mínima</t>
   </si>
 </sst>
 </file>
@@ -728,136 +737,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
     <dxf>
@@ -880,10 +759,140 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1034,7 +1043,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,7 +1139,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,8 +2050,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5F7D2BE3-6EFC-48BE-8EDA-A36D9ADF5C19}" name="Columna1"/>
     <tableColumn id="2" xr3:uid="{AD2F2805-F28A-48A9-9F11-91DACF5006C3}" name="Columna2"/>
-    <tableColumn id="3" xr3:uid="{7CA8D900-196F-4554-8988-8B2A8D04D8ED}" name="Columna3" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{1B170FC1-03D9-49A7-B3BB-6F9A47D3EB2A}" name="Completado" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{7CA8D900-196F-4554-8988-8B2A8D04D8ED}" name="Columna3" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{1B170FC1-03D9-49A7-B3BB-6F9A47D3EB2A}" name="Completado" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2053,8 +2062,8 @@
   <autoFilter ref="A1:E32" xr:uid="{AE16E7A3-A05F-4E67-96A4-32ADB2994F56}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{03B61998-53E0-4293-AB63-FD751979E748}" name="Repaso"/>
-    <tableColumn id="2" xr3:uid="{943925B6-C42F-404B-BDD7-034EE9E9F466}" name="Completado" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{7325186A-CC48-457C-850D-14FBB3BB8D58}" name="Fecha" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{943925B6-C42F-404B-BDD7-034EE9E9F466}" name="Completado" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{7325186A-CC48-457C-850D-14FBB3BB8D58}" name="Fecha" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{E6865B7A-6755-4139-A370-D89B19B1607E}" name="Anotaciones"/>
     <tableColumn id="5" xr3:uid="{E366F3ED-7D01-48C1-B799-FB30B3399D8E}" name="ultima pág"/>
   </tableColumns>
@@ -2386,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE1A602-E64E-4278-BA69-D519A20AD415}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,7 +2440,7 @@
       </c>
       <c r="H2">
         <f>SUM(E:E)</f>
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2452,7 +2461,7 @@
       </c>
       <c r="H3">
         <f>H5-H2</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,7 +2496,7 @@
       </c>
       <c r="H5">
         <f>MAX(A:A)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2508,7 +2517,7 @@
       </c>
       <c r="H6">
         <f>(H2/H5)*100</f>
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2529,7 +2538,7 @@
       </c>
       <c r="H7">
         <f>100-H6</f>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3095,7 +3104,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" s="2">
         <v>44484</v>
@@ -3112,7 +3121,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" s="2">
         <v>44484</v>
@@ -3152,9 +3161,11 @@
       <c r="C44" s="2">
         <v>44492</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,7 +3173,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C45" s="2">
         <v>44494</v>
@@ -3179,14 +3190,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" s="2">
         <v>44492</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3194,14 +3207,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C47" s="2">
         <v>44492</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3209,59 +3224,84 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C48" s="2">
         <v>44492</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="B49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="2">
+        <v>44864</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="B50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="2">
+        <v>44864</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C51" s="2">
-        <v>44492</v>
-      </c>
-      <c r="D51" s="3"/>
+        <v>44864</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C52" s="2">
-        <v>44492</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>44864</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3303,37 +3343,37 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
       <formula>"'x'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D55">
-    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="46" priority="4" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D30 A31:B33 D31:D33 A34:A55">
-    <cfRule type="containsText" dxfId="41" priority="3" operator="containsText" text="x$D:$D">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="x$D:$D">
       <formula>NOT(ISERROR(SEARCH("x$D:$D",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C35">
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="x$D:$D">
+    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="x$D:$D">
       <formula>NOT(ISERROR(SEARCH("x$D:$D",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C33">
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="x$D:$D">
+    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="x$D:$D">
       <formula>NOT(ISERROR(SEARCH("x$D:$D",C31)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3374,7 +3414,7 @@
         <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3567,17 +3607,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B20">
-    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="40" priority="3" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B20">
-    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B20">
-    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="x$D:$D">
+    <cfRule type="containsText" dxfId="38" priority="1" operator="containsText" text="x$D:$D">
       <formula>NOT(ISERROR(SEARCH("x$D:$D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3615,7 +3655,7 @@
         <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3939,17 +3979,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B44">
-    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B44">
-    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="36" priority="5" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B44">
-    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="x$D:$D">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="x$D:$D">
       <formula>NOT(ISERROR(SEARCH("x$D:$D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4032,7 +4072,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1">
         <v>44573</v>
@@ -4046,7 +4086,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="1">
         <v>44573</v>
@@ -4180,7 +4220,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -4189,7 +4229,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -4477,7 +4517,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4534,7 +4574,7 @@
         <v>44896</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>30</v>
@@ -4544,6 +4584,12 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <v>44864</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4612,7 @@
         <v>44512</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="8"/>
     </row>
@@ -4575,7 +4621,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="8"/>
     </row>

</xml_diff>